<commit_message>
Actualizacion de proyecto, se agrega modulo persistencia, cov_monitoreo
</commit_message>
<xml_diff>
--- a/documentation/test_plan.xlsx
+++ b/documentation/test_plan.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="TEST_CASE" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -85,7 +85,7 @@
     <t xml:space="preserve">T_NORMAL_B</t>
   </si>
   <si>
-    <t xml:space="preserve">Estado normal [180 a 250]</t>
+    <t xml:space="preserve">Estado normal [180 a 259]</t>
   </si>
   <si>
     <t xml:space="preserve">Random b_normal</t>
@@ -100,7 +100,7 @@
     <t xml:space="preserve">T_NORMAL_A</t>
   </si>
   <si>
-    <t xml:space="preserve">Estado normal persistente [180 a 250]</t>
+    <t xml:space="preserve">Estado normal persistente [180 a 259]</t>
   </si>
   <si>
     <t xml:space="preserve">Random a_normal_persistente </t>
@@ -298,6 +298,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -432,7 +433,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -629,18 +630,18 @@
   </sheetPr>
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="98" zoomScaleNormal="98" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="92" zoomScaleNormal="92" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="7.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="23.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="51.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="57.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="39.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="37.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="59.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="24.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="16.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="19.2"/>

</xml_diff>